<commit_message>
finish with update user roles from Aperio
</commit_message>
<xml_diff>
--- a/Scanorders2/src/Oleg/OrderformBundle/Helper/users.xlsx
+++ b/Scanorders2/src/Oleg/OrderformBundle/Helper/users.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oli2002\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
   </bookViews>
@@ -15,7 +10,7 @@
     <sheet name="owssvr.dll" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="owssvr.dll" localSheetId="0" hidden="1">owssvr.dll!$A$1:$O$173</definedName>
+    <definedName name="owssvr.dll" localSheetId="0" hidden="1">owssvr.dll!$A$1:$O$174</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -30,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2090" uniqueCount="971">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2093" uniqueCount="974">
   <si>
     <t>A</t>
   </si>
@@ -2943,13 +2938,22 @@
   </si>
   <si>
     <t>C-312</t>
+  </si>
+  <si>
+    <t>Oleg</t>
+  </si>
+  <si>
+    <t>Software Engineer</t>
+  </si>
+  <si>
+    <t>oli2002@med.cornell.edu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3080,6 +3084,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3382,7 +3394,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -3425,14 +3437,16 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -3466,6 +3480,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -3573,8 +3588,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_owssvr.dll" displayName="Table_owssvr.dll" ref="A1:O173" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:O173"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_owssvr.dll" displayName="Table_owssvr.dll" ref="A1:O174" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:O174"/>
   <tableColumns count="15">
     <tableColumn id="1" uniqueName="A" name="A" queryTableFieldId="1" dataDxfId="14"/>
     <tableColumn id="2" uniqueName="Primary_x005f_x0020_Group" name="Primary Group" queryTableFieldId="2" dataDxfId="13"/>
@@ -3851,7 +3866,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3859,10 +3874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O173"/>
+  <dimension ref="A1:O174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L115" sqref="L115"/>
+    <sheetView tabSelected="1" topLeftCell="G159" workbookViewId="0">
+      <selection activeCell="O174" sqref="O174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11335,7 +11350,7 @@
       <c r="K173" s="2" t="s">
         <v>970</v>
       </c>
-      <c r="L173" s="2" t="s">
+      <c r="L173" s="4" t="s">
         <v>967</v>
       </c>
       <c r="M173" s="2" t="s">
@@ -11348,10 +11363,37 @@
         <v>23</v>
       </c>
     </row>
+    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A174" s="1"/>
+      <c r="B174" s="2"/>
+      <c r="C174" s="3"/>
+      <c r="D174" s="2"/>
+      <c r="E174" s="2"/>
+      <c r="F174" s="2"/>
+      <c r="G174" s="2" t="s">
+        <v>971</v>
+      </c>
+      <c r="H174" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="I174" s="2"/>
+      <c r="J174" s="2"/>
+      <c r="K174" s="2"/>
+      <c r="L174" s="4" t="s">
+        <v>973</v>
+      </c>
+      <c r="M174" s="2"/>
+      <c r="N174" s="2"/>
+      <c r="O174" s="2"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L174" r:id="rId1"/>
+    <hyperlink ref="L173" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>